<commit_message>
Adding in check for empty import, turn off az copy
</commit_message>
<xml_diff>
--- a/Scan.xlsx
+++ b/Scan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects-teamhbs\files-o365-readiness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1519E7-01FE-4E21-BB24-5A602A1DE922}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7989731A-0329-40F2-AB13-62D32B354D08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>SourceDirectory</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>\\myfileshare\jbaldwin$\</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -872,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,6 +911,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{51946B69-1A01-478D-A67F-9688418E3279}"/>

</xml_diff>